<commit_message>
uses spread and price
</commit_message>
<xml_diff>
--- a/outputs/RESULTS MAArgentic CLO Case A.xlsx
+++ b/outputs/RESULTS MAArgentic CLO Case A.xlsx
@@ -17,132 +17,102 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
-  <si>
-    <t>[3.474-3.501]</t>
-  </si>
-  <si>
-    <t>[3.501-3.527]</t>
-  </si>
-  <si>
-    <t>[3.527-3.553]</t>
-  </si>
-  <si>
-    <t>[3.553-3.579]</t>
-  </si>
-  <si>
-    <t>[3.579-3.606]</t>
-  </si>
-  <si>
-    <t>[3.606-3.632]</t>
-  </si>
-  <si>
-    <t>[3.632-3.658]</t>
-  </si>
-  <si>
-    <t>[3.658-3.684]</t>
-  </si>
-  <si>
-    <t>[3.684-3.711]</t>
-  </si>
-  <si>
-    <t>[3.711-3.737]</t>
-  </si>
-  <si>
-    <t>[3.737-3.763]</t>
-  </si>
-  <si>
-    <t>[3.763-3.789]</t>
-  </si>
-  <si>
-    <t>[3.789-3.816]</t>
-  </si>
-  <si>
-    <t>[3.816-3.842]</t>
-  </si>
-  <si>
-    <t>[11.45-11.57]</t>
-  </si>
-  <si>
-    <t>[11.57-11.7]</t>
-  </si>
-  <si>
-    <t>[11.7-11.82]</t>
-  </si>
-  <si>
-    <t>[11.82-11.94]</t>
-  </si>
-  <si>
-    <t>[11.94-12.06]</t>
-  </si>
-  <si>
-    <t>[12.06-12.18]</t>
-  </si>
-  <si>
-    <t>[12.18-12.3]</t>
-  </si>
-  <si>
-    <t>[12.3-12.43]</t>
-  </si>
-  <si>
-    <t>[12.43-12.55]</t>
-  </si>
-  <si>
-    <t>[12.55-12.67]</t>
-  </si>
-  <si>
-    <t>[12.67-12.79]</t>
-  </si>
-  <si>
-    <t>[12.79-12.91]</t>
-  </si>
-  <si>
-    <t>[12.91-13.04]</t>
-  </si>
-  <si>
-    <t>[13.04-13.16]</t>
-  </si>
-  <si>
-    <t>[80.56-80.67]</t>
-  </si>
-  <si>
-    <t>[80.67-80.78]</t>
-  </si>
-  <si>
-    <t>[80.78-80.88]</t>
-  </si>
-  <si>
-    <t>[80.88-80.99]</t>
-  </si>
-  <si>
-    <t>[80.99-81.1]</t>
-  </si>
-  <si>
-    <t>[81.1-81.21]</t>
-  </si>
-  <si>
-    <t>[81.21-81.32]</t>
-  </si>
-  <si>
-    <t>[81.32-81.43]</t>
-  </si>
-  <si>
-    <t>[81.43-81.53]</t>
-  </si>
-  <si>
-    <t>[81.53-81.64]</t>
-  </si>
-  <si>
-    <t>[81.64-81.75]</t>
-  </si>
-  <si>
-    <t>[81.75-81.86]</t>
-  </si>
-  <si>
-    <t>[81.86-81.97]</t>
-  </si>
-  <si>
-    <t>[81.97-82.07]</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+  <si>
+    <t>[3.667-3.668]</t>
+  </si>
+  <si>
+    <t>[3.668-3.67]</t>
+  </si>
+  <si>
+    <t>[3.67-3.671]</t>
+  </si>
+  <si>
+    <t>[3.671-3.673]</t>
+  </si>
+  <si>
+    <t>[3.673-3.674]</t>
+  </si>
+  <si>
+    <t>[3.674-3.675]</t>
+  </si>
+  <si>
+    <t>[3.675-3.677]</t>
+  </si>
+  <si>
+    <t>[3.677-3.678]</t>
+  </si>
+  <si>
+    <t>[3.678-3.68]</t>
+  </si>
+  <si>
+    <t>[3.68-3.681]</t>
+  </si>
+  <si>
+    <t>[3.681-3.683]</t>
+  </si>
+  <si>
+    <t>[3.683-3.684]</t>
+  </si>
+  <si>
+    <t>[3.684-3.685]</t>
+  </si>
+  <si>
+    <t>[3.685-3.687]</t>
+  </si>
+  <si>
+    <t>[12.16-12.17]</t>
+  </si>
+  <si>
+    <t>[12.17-12.17]</t>
+  </si>
+  <si>
+    <t>[12.17-12.18]</t>
+  </si>
+  <si>
+    <t>[12.18-12.19]</t>
+  </si>
+  <si>
+    <t>[12.19-12.2]</t>
+  </si>
+  <si>
+    <t>[12.2-12.2]</t>
+  </si>
+  <si>
+    <t>[12.2-12.21]</t>
+  </si>
+  <si>
+    <t>[12.21-12.22]</t>
+  </si>
+  <si>
+    <t>[12.22-12.22]</t>
+  </si>
+  <si>
+    <t>[12.22-12.23]</t>
+  </si>
+  <si>
+    <t>[12.23-12.24]</t>
+  </si>
+  <si>
+    <t>[12.24-12.25]</t>
+  </si>
+  <si>
+    <t>[12.25-12.25]</t>
+  </si>
+  <si>
+    <t>[12.25-12.26]</t>
+  </si>
+  <si>
+    <t>[81.47-81.48]</t>
+  </si>
+  <si>
+    <t>[81.48-81.48]</t>
+  </si>
+  <si>
+    <t>[81.48-81.49]</t>
+  </si>
+  <si>
+    <t>[81.49-81.49]</t>
   </si>
 </sst>
 </file>
@@ -248,31 +218,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>28</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>29</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -287,28 +257,28 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -435,46 +405,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[3.474-3.501]</c:v>
+                  <c:v>[3.667-3.668]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[3.501-3.527]</c:v>
+                  <c:v>[3.668-3.67]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[3.527-3.553]</c:v>
+                  <c:v>[3.67-3.671]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[3.553-3.579]</c:v>
+                  <c:v>[3.671-3.673]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[3.579-3.606]</c:v>
+                  <c:v>[3.673-3.674]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[3.606-3.632]</c:v>
+                  <c:v>[3.674-3.675]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[3.632-3.658]</c:v>
+                  <c:v>[3.675-3.677]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[3.658-3.684]</c:v>
+                  <c:v>[3.677-3.678]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[3.684-3.711]</c:v>
+                  <c:v>[3.678-3.68]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[3.711-3.737]</c:v>
+                  <c:v>[3.68-3.681]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[3.737-3.763]</c:v>
+                  <c:v>[3.681-3.683]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[3.763-3.789]</c:v>
+                  <c:v>[3.683-3.684]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[3.789-3.816]</c:v>
+                  <c:v>[3.684-3.685]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[3.816-3.842]</c:v>
+                  <c:v>[3.685-3.687]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -486,46 +456,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>11</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>17</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -662,46 +632,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[11.45-11.57]</c:v>
+                  <c:v>[12.16-12.17]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[11.57-11.7]</c:v>
+                  <c:v>[12.17-12.17]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[11.7-11.82]</c:v>
+                  <c:v>[12.17-12.18]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[11.82-11.94]</c:v>
+                  <c:v>[12.18-12.19]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[11.94-12.06]</c:v>
+                  <c:v>[12.19-12.2]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[12.06-12.18]</c:v>
+                  <c:v>[12.2-12.2]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[12.18-12.3]</c:v>
+                  <c:v>[12.2-12.21]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[12.3-12.43]</c:v>
+                  <c:v>[12.21-12.22]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[12.43-12.55]</c:v>
+                  <c:v>[12.22-12.22]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[12.55-12.67]</c:v>
+                  <c:v>[12.22-12.23]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[12.67-12.79]</c:v>
+                  <c:v>[12.23-12.24]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[12.79-12.91]</c:v>
+                  <c:v>[12.24-12.25]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[12.91-13.04]</c:v>
+                  <c:v>[12.25-12.25]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[13.04-13.16]</c:v>
+                  <c:v>[12.25-12.26]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -713,46 +683,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>18</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -889,46 +859,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[80.56-80.67]</c:v>
+                  <c:v>[81.47-81.48]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[80.67-80.78]</c:v>
+                  <c:v>[81.48-81.48]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[80.78-80.88]</c:v>
+                  <c:v>[81.48-81.48]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[80.88-80.99]</c:v>
+                  <c:v>[81.48-81.48]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[80.99-81.1]</c:v>
+                  <c:v>[81.48-81.48]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[81.1-81.21]</c:v>
+                  <c:v>[81.48-81.48]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[81.21-81.32]</c:v>
+                  <c:v>[81.48-81.48]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[81.32-81.43]</c:v>
+                  <c:v>[81.48-81.49]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[81.43-81.53]</c:v>
+                  <c:v>[81.49-81.49]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[81.53-81.64]</c:v>
+                  <c:v>[81.49-81.49]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[81.64-81.75]</c:v>
+                  <c:v>[81.49-81.49]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[81.75-81.86]</c:v>
+                  <c:v>[81.49-81.49]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[81.86-81.97]</c:v>
+                  <c:v>[81.49-81.49]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[81.97-82.07]</c:v>
+                  <c:v>[81.49-81.49]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -940,46 +910,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>15</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1509,7 +1479,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -1517,26 +1487,26 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1544,44 +1514,44 @@
         <v>24</v>
       </c>
       <c r="B5">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7">
-        <v>31</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1603,7 +1573,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1611,7 +1581,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1619,7 +1589,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1627,7 +1597,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1635,7 +1605,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1643,7 +1613,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1651,7 +1621,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1659,7 +1629,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1667,7 +1637,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1675,7 +1645,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1683,7 +1653,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1699,7 +1669,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1707,7 +1677,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1729,7 +1699,7 @@
         <v>14</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1737,7 +1707,7 @@
         <v>15</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1753,7 +1723,7 @@
         <v>17</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1761,7 +1731,7 @@
         <v>18</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1769,7 +1739,7 @@
         <v>19</v>
       </c>
       <c r="B6">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1777,7 +1747,7 @@
         <v>20</v>
       </c>
       <c r="B7">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1785,7 +1755,7 @@
         <v>21</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1793,7 +1763,7 @@
         <v>22</v>
       </c>
       <c r="B9">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1801,7 +1771,7 @@
         <v>23</v>
       </c>
       <c r="B10">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1809,7 +1779,7 @@
         <v>24</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1817,7 +1787,7 @@
         <v>25</v>
       </c>
       <c r="B12">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1825,7 +1795,7 @@
         <v>26</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1833,7 +1803,7 @@
         <v>27</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1855,7 +1825,7 @@
         <v>28</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1868,98 +1838,98 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B7">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B8">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B9">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B10">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B11">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B12">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B14">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed error in current clo size calculation, now only adds up offered tranches
</commit_message>
<xml_diff>
--- a/outputs/RESULTS MAArgentic CLO Case A.xlsx
+++ b/outputs/RESULTS MAArgentic CLO Case A.xlsx
@@ -19,130 +19,130 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
-    <t>[3.61-3.616]</t>
-  </si>
-  <si>
-    <t>[3.616-3.622]</t>
-  </si>
-  <si>
-    <t>[3.622-3.628]</t>
-  </si>
-  <si>
-    <t>[3.628-3.634]</t>
-  </si>
-  <si>
-    <t>[3.634-3.639]</t>
-  </si>
-  <si>
-    <t>[3.639-3.645]</t>
-  </si>
-  <si>
-    <t>[3.645-3.651]</t>
-  </si>
-  <si>
-    <t>[3.651-3.657]</t>
-  </si>
-  <si>
-    <t>[3.657-3.663]</t>
-  </si>
-  <si>
-    <t>[3.663-3.669]</t>
-  </si>
-  <si>
-    <t>[3.669-3.675]</t>
-  </si>
-  <si>
-    <t>[3.675-3.68]</t>
-  </si>
-  <si>
-    <t>[3.68-3.686]</t>
-  </si>
-  <si>
-    <t>[3.686-3.692]</t>
-  </si>
-  <si>
-    <t>[12.13-12.16]</t>
-  </si>
-  <si>
-    <t>[12.16-12.19]</t>
-  </si>
-  <si>
-    <t>[12.19-12.21]</t>
-  </si>
-  <si>
-    <t>[12.21-12.24]</t>
-  </si>
-  <si>
-    <t>[12.24-12.27]</t>
-  </si>
-  <si>
-    <t>[12.27-12.29]</t>
-  </si>
-  <si>
-    <t>[12.29-12.32]</t>
-  </si>
-  <si>
-    <t>[12.32-12.35]</t>
-  </si>
-  <si>
-    <t>[12.35-12.38]</t>
-  </si>
-  <si>
-    <t>[12.38-12.4]</t>
-  </si>
-  <si>
-    <t>[12.4-12.43]</t>
-  </si>
-  <si>
-    <t>[12.43-12.46]</t>
-  </si>
-  <si>
-    <t>[12.46-12.48]</t>
-  </si>
-  <si>
-    <t>[12.48-12.51]</t>
-  </si>
-  <si>
-    <t>[81.08-81.11]</t>
-  </si>
-  <si>
-    <t>[81.11-81.14]</t>
-  </si>
-  <si>
-    <t>[81.14-81.17]</t>
-  </si>
-  <si>
-    <t>[81.17-81.2]</t>
-  </si>
-  <si>
-    <t>[81.2-81.23]</t>
-  </si>
-  <si>
-    <t>[81.23-81.26]</t>
-  </si>
-  <si>
-    <t>[81.26-81.29]</t>
-  </si>
-  <si>
-    <t>[81.29-81.32]</t>
-  </si>
-  <si>
-    <t>[81.32-81.35]</t>
-  </si>
-  <si>
-    <t>[81.35-81.38]</t>
-  </si>
-  <si>
-    <t>[81.38-81.41]</t>
-  </si>
-  <si>
-    <t>[81.41-81.44]</t>
-  </si>
-  <si>
-    <t>[81.44-81.47]</t>
-  </si>
-  <si>
-    <t>[81.47-81.5]</t>
+    <t>[3.539-3.547]</t>
+  </si>
+  <si>
+    <t>[3.547-3.556]</t>
+  </si>
+  <si>
+    <t>[3.556-3.564]</t>
+  </si>
+  <si>
+    <t>[3.564-3.573]</t>
+  </si>
+  <si>
+    <t>[3.573-3.581]</t>
+  </si>
+  <si>
+    <t>[3.581-3.59]</t>
+  </si>
+  <si>
+    <t>[3.59-3.598]</t>
+  </si>
+  <si>
+    <t>[3.598-3.607]</t>
+  </si>
+  <si>
+    <t>[3.607-3.615]</t>
+  </si>
+  <si>
+    <t>[3.615-3.623]</t>
+  </si>
+  <si>
+    <t>[3.623-3.632]</t>
+  </si>
+  <si>
+    <t>[3.632-3.64]</t>
+  </si>
+  <si>
+    <t>[3.64-3.649]</t>
+  </si>
+  <si>
+    <t>[3.649-3.657]</t>
+  </si>
+  <si>
+    <t>[12.3-12.34]</t>
+  </si>
+  <si>
+    <t>[12.34-12.38]</t>
+  </si>
+  <si>
+    <t>[12.38-12.42]</t>
+  </si>
+  <si>
+    <t>[12.42-12.46]</t>
+  </si>
+  <si>
+    <t>[12.46-12.5]</t>
+  </si>
+  <si>
+    <t>[12.5-12.54]</t>
+  </si>
+  <si>
+    <t>[12.54-12.58]</t>
+  </si>
+  <si>
+    <t>[12.58-12.62]</t>
+  </si>
+  <si>
+    <t>[12.62-12.66]</t>
+  </si>
+  <si>
+    <t>[12.66-12.7]</t>
+  </si>
+  <si>
+    <t>[12.7-12.74]</t>
+  </si>
+  <si>
+    <t>[12.74-12.78]</t>
+  </si>
+  <si>
+    <t>[12.78-12.82]</t>
+  </si>
+  <si>
+    <t>[12.82-12.86]</t>
+  </si>
+  <si>
+    <t>[81.83-81.84]</t>
+  </si>
+  <si>
+    <t>[81.84-81.85]</t>
+  </si>
+  <si>
+    <t>[81.85-81.86]</t>
+  </si>
+  <si>
+    <t>[81.86-81.86]</t>
+  </si>
+  <si>
+    <t>[81.86-81.87]</t>
+  </si>
+  <si>
+    <t>[81.87-81.88]</t>
+  </si>
+  <si>
+    <t>[81.88-81.89]</t>
+  </si>
+  <si>
+    <t>[81.89-81.89]</t>
+  </si>
+  <si>
+    <t>[81.89-81.9]</t>
+  </si>
+  <si>
+    <t>[81.9-81.91]</t>
+  </si>
+  <si>
+    <t>[81.91-81.92]</t>
+  </si>
+  <si>
+    <t>[81.92-81.92]</t>
+  </si>
+  <si>
+    <t>[81.92-81.93]</t>
+  </si>
+  <si>
+    <t>[81.93-81.94]</t>
   </si>
 </sst>
 </file>
@@ -435,46 +435,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[3.61-3.616]</c:v>
+                  <c:v>[3.539-3.547]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[3.616-3.622]</c:v>
+                  <c:v>[3.547-3.556]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[3.622-3.628]</c:v>
+                  <c:v>[3.556-3.564]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[3.628-3.634]</c:v>
+                  <c:v>[3.564-3.573]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[3.634-3.639]</c:v>
+                  <c:v>[3.573-3.581]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[3.639-3.645]</c:v>
+                  <c:v>[3.581-3.59]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[3.645-3.651]</c:v>
+                  <c:v>[3.59-3.598]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[3.651-3.657]</c:v>
+                  <c:v>[3.598-3.607]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[3.657-3.663]</c:v>
+                  <c:v>[3.607-3.615]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[3.663-3.669]</c:v>
+                  <c:v>[3.615-3.623]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[3.669-3.675]</c:v>
+                  <c:v>[3.623-3.632]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[3.675-3.68]</c:v>
+                  <c:v>[3.632-3.64]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[3.68-3.686]</c:v>
+                  <c:v>[3.64-3.649]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[3.686-3.692]</c:v>
+                  <c:v>[3.649-3.657]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -662,46 +662,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[12.13-12.16]</c:v>
+                  <c:v>[12.3-12.34]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[12.16-12.19]</c:v>
+                  <c:v>[12.34-12.38]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[12.19-12.21]</c:v>
+                  <c:v>[12.38-12.42]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[12.21-12.24]</c:v>
+                  <c:v>[12.42-12.46]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[12.24-12.27]</c:v>
+                  <c:v>[12.46-12.5]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[12.27-12.29]</c:v>
+                  <c:v>[12.5-12.54]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[12.29-12.32]</c:v>
+                  <c:v>[12.54-12.58]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[12.32-12.35]</c:v>
+                  <c:v>[12.58-12.62]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[12.35-12.38]</c:v>
+                  <c:v>[12.62-12.66]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[12.38-12.4]</c:v>
+                  <c:v>[12.66-12.7]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[12.4-12.43]</c:v>
+                  <c:v>[12.7-12.74]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[12.43-12.46]</c:v>
+                  <c:v>[12.74-12.78]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[12.46-12.48]</c:v>
+                  <c:v>[12.78-12.82]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[12.48-12.51]</c:v>
+                  <c:v>[12.82-12.86]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -746,10 +746,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -889,46 +889,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[81.08-81.11]</c:v>
+                  <c:v>[81.83-81.84]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[81.11-81.14]</c:v>
+                  <c:v>[81.84-81.85]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[81.14-81.17]</c:v>
+                  <c:v>[81.85-81.86]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[81.17-81.2]</c:v>
+                  <c:v>[81.86-81.86]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[81.2-81.23]</c:v>
+                  <c:v>[81.86-81.87]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[81.23-81.26]</c:v>
+                  <c:v>[81.87-81.88]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[81.26-81.29]</c:v>
+                  <c:v>[81.88-81.89]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[81.29-81.32]</c:v>
+                  <c:v>[81.89-81.89]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[81.32-81.35]</c:v>
+                  <c:v>[81.89-81.9]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[81.35-81.38]</c:v>
+                  <c:v>[81.9-81.91]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[81.38-81.41]</c:v>
+                  <c:v>[81.91-81.92]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[81.41-81.44]</c:v>
+                  <c:v>[81.92-81.92]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[81.44-81.47]</c:v>
+                  <c:v>[81.92-81.93]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[81.47-81.5]</c:v>
+                  <c:v>[81.93-81.94]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -940,11 +940,11 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
@@ -976,10 +976,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1817,7 +1817,7 @@
         <v>25</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1825,7 +1825,7 @@
         <v>26</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1855,7 +1855,7 @@
         <v>28</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1863,7 +1863,7 @@
         <v>29</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1951,7 +1951,7 @@
         <v>40</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1959,7 +1959,7 @@
         <v>41</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>